<commit_message>
php code for getting student result + some bug fixes
added seat no column in database and appropriate code to import it
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\cb\SIMPLE_RESULT_MANAGMENT_SYSTEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0501C2AD-8A31-4EC1-B6CC-58DA9703A1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A534D5FC-67AC-4810-B666-860F9D8E447A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{56547FED-2B71-4427-8F7D-818A78528850}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>STUDENT_NAME</t>
   </si>
@@ -92,6 +92,33 @@
   </si>
   <si>
     <t>MOTHER NAME</t>
+  </si>
+  <si>
+    <t>SEAT NO:</t>
+  </si>
+  <si>
+    <t>s1</t>
+  </si>
+  <si>
+    <t>s2</t>
+  </si>
+  <si>
+    <t>s3</t>
+  </si>
+  <si>
+    <t>s4</t>
+  </si>
+  <si>
+    <t>s5</t>
+  </si>
+  <si>
+    <t>s6</t>
+  </si>
+  <si>
+    <t>s7</t>
+  </si>
+  <si>
+    <t>s8</t>
   </si>
 </sst>
 </file>
@@ -456,18 +483,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A841782A-9C55-4189-AF5C-FAF98F02A187}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="29" customWidth="1"/>
+    <col min="2" max="3" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -475,17 +502,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="1">
-        <v>30</v>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>16</v>
       </c>
       <c r="D3" s="1">
         <v>30</v>
@@ -499,211 +523,241 @@
       <c r="G3" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
         <v>30</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>25</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>12</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>25</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
         <v>23</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>12</v>
       </c>
-      <c r="E6">
-        <v>16</v>
-      </c>
       <c r="F6">
+        <v>16</v>
+      </c>
+      <c r="G6">
         <v>28</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C7">
-        <v>16</v>
+      <c r="C7" t="s">
+        <v>8</v>
       </c>
       <c r="D7">
+        <v>16</v>
+      </c>
+      <c r="E7">
         <v>23</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>20</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>24</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C8">
+      <c r="C8" t="s">
         <v>9</v>
       </c>
       <c r="D8">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E8">
+        <v>16</v>
+      </c>
+      <c r="F8">
         <v>24</v>
       </c>
-      <c r="F8">
-        <v>16</v>
-      </c>
       <c r="G8">
+        <v>16</v>
+      </c>
+      <c r="H8">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9">
         <v>23</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>9</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>28</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>20</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10">
         <v>9</v>
       </c>
-      <c r="D10">
-        <v>16</v>
-      </c>
       <c r="E10">
         <v>16</v>
       </c>
       <c r="F10">
+        <v>16</v>
+      </c>
+      <c r="G10">
         <v>24</v>
       </c>
-      <c r="G10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11">
         <v>9</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>20</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>24</v>
       </c>
-      <c r="F11">
-        <v>16</v>
-      </c>
       <c r="G11">
+        <v>16</v>
+      </c>
+      <c r="H11">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12">
         <v>23</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>24</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>15</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>20</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>30</v>
       </c>
     </row>

</xml_diff>